<commit_message>
yeah some nth commit
</commit_message>
<xml_diff>
--- a/static/registrations.xlsx
+++ b/static/registrations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -542,9 +542,29 @@
         <v/>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>AGNIVA BHATTACHARJEE</v>
+      </c>
+      <c r="B8" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="C8" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2020</v>
+      </c>
+      <c r="E8" t="str">
+        <v>3ba20b57-9c39-4880-8ae1-203fa0db0544</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wanted to check the template width and height
</commit_message>
<xml_diff>
--- a/static/registrations.xlsx
+++ b/static/registrations.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -582,9 +582,49 @@
         <v/>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Shriparna Gupta</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2001shriparna@gmail.com</v>
+      </c>
+      <c r="C10" t="str">
+        <v>8420845844</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2020</v>
+      </c>
+      <c r="E10" t="str">
+        <v>2969cc7d-a02b-426b-88d7-a46885ced627</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>AGNIVA BHATTACHARJEE</v>
+      </c>
+      <c r="B11" t="str">
+        <v>imagniva007@gmail.com</v>
+      </c>
+      <c r="C11" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="D11" t="str">
+        <v>2020</v>
+      </c>
+      <c r="E11" t="str">
+        <v>c614ae38-316f-4b39-a47a-d16587c2f533</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>